<commit_message>
Changes to integrate Contact page Test Scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestData.xlsx
+++ b/src/test/resources/Data/TestData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCAF3B9-70EE-47CA-AFF8-D1E299EF4641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -79,13 +78,31 @@
   </si>
   <si>
     <t>ACC</t>
+  </si>
+  <si>
+    <t>nature</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>Test_Enginner</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>Tendulkar</t>
+  </si>
+  <si>
+    <t>TC05_create_contact_with_mandatory_fields</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,20 +188,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -222,7 +247,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -256,6 +281,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -290,9 +316,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,20 +492,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -503,8 +531,11 @@
       <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -519,8 +550,9 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -535,8 +567,9 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -557,9 +590,10 @@
         <v>14</v>
       </c>
       <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -568,7 +602,7 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="1"/>
@@ -577,33 +611,37 @@
       <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>